<commit_message>
:art: changed export file to accommodate changed semester and lehrjahr, and Ascend sorted
</commit_message>
<xml_diff>
--- a/praktikumsplaner-backend/src/main/resources-non-filtered/templates/ITM_IT_POR.xlsx
+++ b/praktikumsplaner-backend/src/main/resources-non-filtered/templates/ITM_IT_POR.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31B77366-CE95-4FAA-A324-450F7AE35A23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C25D0B6-ED06-441F-977A-64C0969900F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-5550" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{ECF369DD-E939-4FB1-9EAA-B3EEB7A3D364}"/>
   </bookViews>
@@ -79,10 +79,6 @@
   </si>
   <si>
     <t>Programmierkenntnisse</t>
-  </si>
-  <si>
-    <t>Ausbildungsjahr
-(optional)</t>
   </si>
   <si>
     <t>Ausbildungsart</t>
@@ -414,205 +410,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>Hier können Sie (optional) eine Präferenz bzgl. Studiensemester angeben.
--</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> ab 1. Semester
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> ab 2. Semester
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> ab 3. Semester
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> ab 4. Semester
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> ab 5. Semester</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
--</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> ab 6. Semester</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Hier können Sie (optional) eine Präferenz bzgl. </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Ausbildungsjahr </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">angeben.
-- </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>ab 1. Jahr</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-- </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>ab 2. Jahr</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="0" tint="-0.499984740745262"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-- </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>ab 3. Jahr</t>
-    </r>
-  </si>
-  <si>
     <t>Programmierkenntnisse (optional)</t>
   </si>
   <si>
@@ -712,6 +509,208 @@
   <si>
     <t>Hier finden Sie den Namen der aktuell auf diesen PP zugewiesenen NWK. 
 Namentliche Anforderungen oder Verlängerungen für die Zukunft sind bei Hinweisen einzutragen.</t>
+  </si>
+  <si>
+    <r>
+      <t>Hier können Sie Präferenzen bzgl. Studiensemester angeben.
+-</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 1. Semester
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 2. Semester
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 3. Semester
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 4. Semester
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>-</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 5. Semester</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+-</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 6. Semester</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Hier können Sie Präferenzen bzgl. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Ausbildungsjahr </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">angeben.
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>1. Jahr</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+-</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 2. Jahr</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>3. Jahr</t>
+    </r>
+  </si>
+  <si>
+    <t>Ausbildungsjahr</t>
   </si>
 </sst>
 </file>
@@ -1328,7 +1327,7 @@
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1:O1048576"/>
+      <selection pane="bottomLeft" activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.09765625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1364,25 +1363,25 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>14</v>
+        <v>46</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>9</v>
@@ -1400,79 +1399,79 @@
     <row r="2" spans="1:15" ht="249.6" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="F2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="K2" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>12</v>
       </c>
       <c r="O2" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:15" s="27" customFormat="1" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="24" t="s">
-        <v>21</v>
-      </c>
       <c r="D3" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="24" t="s">
-        <v>31</v>
-      </c>
       <c r="F3" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G3" s="23"/>
       <c r="H3" s="24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I3" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J3" s="24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K3" s="24" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L3" s="28"/>
       <c r="M3" s="28"/>
@@ -1668,197 +1667,101 @@
       <c r="F16" s="4"/>
       <c r="I16" s="4"/>
     </row>
-    <row r="17" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="P17" s="4"/>
-    </row>
-    <row r="18" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="P18" s="4"/>
-    </row>
-    <row r="19" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="P19" s="4"/>
-    </row>
-    <row r="20" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="P20" s="4"/>
-    </row>
-    <row r="21" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="P21" s="4"/>
-    </row>
-    <row r="22" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="I22" s="4"/>
-      <c r="P22" s="4"/>
-    </row>
-    <row r="23" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="I23" s="4"/>
-      <c r="P23" s="4"/>
-    </row>
-    <row r="24" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="I24" s="4"/>
-      <c r="P24" s="4"/>
-    </row>
-    <row r="25" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="I25" s="4"/>
-      <c r="P25" s="4"/>
-    </row>
-    <row r="26" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="I26" s="4"/>
-      <c r="P26" s="4"/>
-    </row>
-    <row r="27" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="I27" s="4"/>
-      <c r="P27" s="4"/>
-    </row>
-    <row r="28" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="I28" s="4"/>
-      <c r="P28" s="4"/>
-    </row>
-    <row r="29" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="I29" s="4"/>
-      <c r="P29" s="4"/>
-    </row>
-    <row r="30" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="I30" s="4"/>
-      <c r="P30" s="4"/>
-    </row>
-    <row r="31" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="I31" s="4"/>
-      <c r="P31" s="4"/>
-    </row>
-    <row r="32" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="I32" s="4"/>
-      <c r="P32" s="4"/>
-    </row>
-    <row r="33" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="I33" s="4"/>
-      <c r="P33" s="4"/>
-    </row>
-    <row r="34" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D34" s="4"/>
-      <c r="F34" s="4"/>
-      <c r="I34" s="4"/>
-      <c r="P34" s="4"/>
-    </row>
-    <row r="35" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="I35" s="4"/>
-      <c r="P35" s="4"/>
-    </row>
-    <row r="36" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D36" s="4"/>
-      <c r="F36" s="4"/>
-      <c r="I36" s="4"/>
-      <c r="P36" s="4"/>
-    </row>
-    <row r="37" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D37" s="4"/>
-      <c r="F37" s="4"/>
-      <c r="I37" s="4"/>
-      <c r="P37" s="4"/>
-    </row>
-    <row r="38" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D38" s="4"/>
-      <c r="F38" s="4"/>
-      <c r="I38" s="4"/>
-      <c r="P38" s="4"/>
-    </row>
-    <row r="39" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D39" s="4"/>
-      <c r="F39" s="4"/>
-      <c r="I39" s="4"/>
-      <c r="P39" s="4"/>
-    </row>
-    <row r="40" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D40" s="4"/>
-      <c r="F40" s="4"/>
-      <c r="I40" s="4"/>
-      <c r="P40" s="4"/>
-    </row>
-    <row r="41" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D41" s="4"/>
-      <c r="F41" s="4"/>
-      <c r="I41" s="4"/>
-      <c r="P41" s="4"/>
-    </row>
-    <row r="42" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D42" s="4"/>
-      <c r="F42" s="4"/>
-      <c r="I42" s="4"/>
-      <c r="P42" s="4"/>
-    </row>
-    <row r="43" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D43" s="4"/>
-      <c r="F43" s="4"/>
-      <c r="I43" s="4"/>
-      <c r="P43" s="4"/>
-    </row>
-    <row r="44" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D44" s="4"/>
-      <c r="F44" s="4"/>
-      <c r="I44" s="4"/>
-      <c r="P44" s="4"/>
-    </row>
-    <row r="45" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D45" s="4"/>
-      <c r="F45" s="4"/>
-      <c r="I45" s="4"/>
-      <c r="P45" s="4"/>
-    </row>
-    <row r="46" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D46" s="4"/>
-      <c r="F46" s="4"/>
-      <c r="I46" s="4"/>
-      <c r="P46" s="4"/>
-    </row>
-    <row r="47" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D47" s="4"/>
-      <c r="F47" s="4"/>
-      <c r="I47" s="4"/>
-      <c r="P47" s="4"/>
-    </row>
-    <row r="48" spans="4:16" x14ac:dyDescent="0.25">
-      <c r="D48" s="4"/>
-      <c r="F48" s="4"/>
-      <c r="I48" s="4"/>
-      <c r="P48" s="4"/>
+    <row r="17" spans="5:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E17"/>
+    </row>
+    <row r="18" spans="5:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E18"/>
+    </row>
+    <row r="19" spans="5:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E19"/>
+    </row>
+    <row r="20" spans="5:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E20"/>
+    </row>
+    <row r="21" spans="5:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E21"/>
+    </row>
+    <row r="22" spans="5:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E22"/>
+    </row>
+    <row r="23" spans="5:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E23"/>
+    </row>
+    <row r="24" spans="5:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E24"/>
+    </row>
+    <row r="25" spans="5:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E25"/>
+    </row>
+    <row r="26" spans="5:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E26"/>
+    </row>
+    <row r="27" spans="5:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E27"/>
+    </row>
+    <row r="28" spans="5:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E28"/>
+    </row>
+    <row r="29" spans="5:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E29"/>
+    </row>
+    <row r="30" spans="5:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E30"/>
+    </row>
+    <row r="31" spans="5:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E31"/>
+    </row>
+    <row r="32" spans="5:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E32"/>
+    </row>
+    <row r="33" spans="5:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E33"/>
+    </row>
+    <row r="34" spans="5:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E34"/>
+    </row>
+    <row r="35" spans="5:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E35"/>
+    </row>
+    <row r="36" spans="5:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E36"/>
+    </row>
+    <row r="37" spans="5:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E37"/>
+    </row>
+    <row r="38" spans="5:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E38"/>
+    </row>
+    <row r="39" spans="5:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E39"/>
+    </row>
+    <row r="40" spans="5:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E40"/>
+    </row>
+    <row r="41" spans="5:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E41"/>
+    </row>
+    <row r="42" spans="5:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E42"/>
+    </row>
+    <row r="43" spans="5:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E43"/>
+    </row>
+    <row r="44" spans="5:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E44"/>
+    </row>
+    <row r="45" spans="5:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E45"/>
+    </row>
+    <row r="46" spans="5:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E46"/>
+    </row>
+    <row r="47" spans="5:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E47"/>
+    </row>
+    <row r="48" spans="5:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="E48"/>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D49" s="4"/>
@@ -5633,7 +5536,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D27" sqref="D27"/>
+      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.09765625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -5669,7 +5572,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>13</v>
@@ -5678,13 +5581,13 @@
         <v>7</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K1" s="3" t="s">
         <v>4</v>
@@ -5702,73 +5605,73 @@
     <row r="2" spans="1:14" ht="302.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="F2" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>42</v>
-      </c>
       <c r="J2" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="M2" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:14" s="27" customFormat="1" ht="46.8" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="24" t="s">
-        <v>21</v>
-      </c>
       <c r="D3" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="24" t="s">
-        <v>31</v>
-      </c>
       <c r="F3" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H3" s="13"/>
       <c r="I3" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J3" s="24" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K3" s="25"/>
       <c r="L3" s="28"/>

</xml_diff>